<commit_message>
Updated HW3 to remove stall with forwarding on the branch instruction
</commit_message>
<xml_diff>
--- a/Assignments/HW3_Matrix.xlsx
+++ b/Assignments/HW3_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\WI2019\Architecture\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481A29CB-DF6C-4F0B-9699-3DDADEBEB18D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09217852-BA9D-4E7C-A4DC-724EEC42E574}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B - No forward" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="41">
   <si>
     <t>Instruction</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Assume branch taken:</t>
   </si>
   <si>
-    <t>8 cycles/loop</t>
-  </si>
-  <si>
     <t>NEXT2</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>x4, loop</t>
+  </si>
+  <si>
+    <t>7 cycles/loop</t>
   </si>
 </sst>
 </file>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,9 +268,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -623,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
@@ -747,7 +744,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="Z2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -764,11 +761,11 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>39</v>
+      <c r="G3" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>4</v>
@@ -791,7 +788,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="Z3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -811,11 +808,11 @@
       <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>39</v>
+      <c r="J4" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>4</v>
@@ -835,7 +832,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="Z4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -896,11 +893,11 @@
       <c r="M6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>39</v>
+      <c r="N6" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>4</v>
@@ -917,47 +914,47 @@
       <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="18" t="s">
+      <c r="C7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="17" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="U7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
+      <c r="R7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -977,14 +974,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="12"/>
+      <c r="Q8" s="11"/>
       <c r="R8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="T8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="U8" s="5"/>
@@ -1009,12 +1006,12 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="12"/>
+      <c r="Q9" s="11"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="U9" s="5"/>
@@ -1346,7 +1343,7 @@
   <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,11 +1519,11 @@
       <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>38</v>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>4</v>
@@ -1584,7 +1581,7 @@
       <c r="S4" s="5"/>
       <c r="V4" s="5"/>
       <c r="AA4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -1622,7 +1619,7 @@
       <c r="S5" s="5"/>
       <c r="V5" s="5"/>
       <c r="AA5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -1658,42 +1655,39 @@
       <c r="R6" s="5"/>
       <c r="V6" s="5"/>
       <c r="AA6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="5"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1708,18 +1702,17 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="L8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1735,16 +1728,15 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="10" t="s">
+      <c r="L9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="9"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1756,21 +1748,22 @@
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="M10" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="N10" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
@@ -1784,7 +1777,6 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1794,25 +1786,26 @@
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>38</v>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
@@ -1824,7 +1817,6 @@
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
       <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1834,33 +1826,33 @@
       <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
+      <c r="P12" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="Q12" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="U12" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1870,33 +1862,33 @@
       <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
+      <c r="Q13" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="R13" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="V13" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="5"/>
-      <c r="AF13" s="5"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1906,81 +1898,77 @@
       <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
+      <c r="R14" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="S14" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="W14" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AF14" s="5"/>
+      <c r="AE14" s="5"/>
     </row>
     <row r="15" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="U15" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="V15" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="W15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="X15" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y15" s="14" t="s">
-        <v>6</v>
-      </c>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="U15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
-      <c r="AE15" s="5"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1988,38 +1976,38 @@
         <v>17</v>
       </c>
       <c r="C16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="X16" s="10" t="s">
+      <c r="T16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16" s="19" t="s">
         <v>19</v>
       </c>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="20"/>
-      <c r="AE16" s="20"/>
-      <c r="AF16" s="20"/>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="5"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -2027,24 +2015,22 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="X17" s="10" t="s">
+      <c r="U17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="19" t="s">
         <v>19</v>
       </c>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="20"/>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2054,29 +2040,29 @@
       <c r="C18" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="V18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="X18" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB18" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
       <c r="AE18" s="5"/>
       <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
@@ -2084,31 +2070,31 @@
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="X19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="Y19" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z19" s="5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AA19" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
       <c r="AE19" s="5"/>
       <c r="AF19" s="5"/>
-      <c r="AG19" s="5"/>
-      <c r="AH19" s="5"/>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="5" t="s">
         <v>11</v>
@@ -2116,28 +2102,28 @@
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
       <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-      <c r="Z20" s="5"/>
+      <c r="Y20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="AA20" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG20" s="5"/>
-      <c r="AH20" s="5"/>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="5" t="s">
         <v>9</v>
@@ -2145,28 +2131,28 @@
       <c r="C21" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
+      <c r="Z21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="AB21" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH21" s="5"/>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AF21" s="5"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
@@ -2174,119 +2160,114 @@
       <c r="C22" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
-      <c r="AA22" s="5"/>
-      <c r="AB22" s="5"/>
+      <c r="AA22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="AC22" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG22" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
       <c r="V23" s="13"/>
       <c r="W23" s="13"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
-      <c r="Z23" s="14"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
-      <c r="AC23" s="14"/>
-      <c r="AD23" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE23" s="14" t="s">
-        <v>14</v>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD23" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE23" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="AF23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG23" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH23" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI23" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="5"/>
       <c r="F24" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
+      <c r="AD24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE24" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="AF24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG24" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ24" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AG24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH24" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="5"/>
+      <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
@@ -2294,29 +2275,23 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AG25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI25" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK25" s="9" t="s">
+      <c r="AE25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI25" s="9" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="AD16:AF16"/>
-    <mergeCell ref="AD17:AF17"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2326,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020A401E-0E1F-4B01-AAD3-33C84EC0B4CF}">
   <dimension ref="A1:AF19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,11 +2464,11 @@
       <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>38</v>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>4</v>
@@ -2620,38 +2595,35 @@
       <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="5"/>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2663,29 +2635,29 @@
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="K8" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="L8" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
@@ -2696,30 +2668,30 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -2729,26 +2701,26 @@
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="N10" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="O10" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="T10" s="5"/>
       <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -2757,23 +2729,23 @@
       <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="O11" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="P11" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2784,75 +2756,71 @@
       <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
+      <c r="P12" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="Q12" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="U12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="AF12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="U13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF13" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="T13" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="U13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="W13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="X13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -2865,28 +2833,28 @@
       <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="R14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="T14" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="W14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="X14" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
       <c r="AF14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -2897,69 +2865,69 @@
       <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="V15" s="12" t="s">
+      <c r="R15" s="5"/>
+      <c r="S15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="V16" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA16" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="Y16" s="5"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="5"/>
     </row>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
+      <c r="U17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="W17" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="AB17" s="5"/>

</xml_diff>

<commit_message>
Fixed flush issue when branch predicts taken
</commit_message>
<xml_diff>
--- a/Assignments/HW3_Matrix.xlsx
+++ b/Assignments/HW3_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\WI2019\Architecture\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09217852-BA9D-4E7C-A4DC-724EEC42E574}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FC52E3-3660-49CA-8394-07D96D30CCB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="41">
   <si>
     <t>Instruction</t>
   </si>
@@ -102,9 +102,6 @@
     <t>NEXT1</t>
   </si>
   <si>
-    <t>&lt;-- Final Cycle for loop</t>
-  </si>
-  <si>
     <t>99 loops @ 8 cycles/loop = 792 cycles</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>7 cycles/loop</t>
+  </si>
+  <si>
+    <t>&lt;-- Final Cycle of loop</t>
   </si>
 </sst>
 </file>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,7 +268,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -276,9 +275,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,7 +763,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="Z2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -761,11 +780,11 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>38</v>
+      <c r="G3" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>4</v>
@@ -788,7 +807,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="Z3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -808,11 +827,11 @@
       <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>38</v>
+      <c r="J4" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>4</v>
@@ -832,7 +851,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="Z4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -893,11 +912,11 @@
       <c r="M6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="11" t="s">
-        <v>38</v>
+      <c r="N6" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>4</v>
@@ -914,47 +933,47 @@
       <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="R7" s="16" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
+      <c r="R7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -974,14 +993,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="11"/>
+      <c r="Q8" s="10"/>
       <c r="R8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="T8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="U8" s="5"/>
@@ -1006,12 +1025,12 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="11"/>
+      <c r="Q9" s="10"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="T9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="U9" s="5"/>
@@ -1519,11 +1538,11 @@
       <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>37</v>
+      <c r="F3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>4</v>
@@ -1581,7 +1600,7 @@
       <c r="S4" s="5"/>
       <c r="V4" s="5"/>
       <c r="AA4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -1619,7 +1638,7 @@
       <c r="S5" s="5"/>
       <c r="V5" s="5"/>
       <c r="AA5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -1655,36 +1674,36 @@
       <c r="R6" s="5"/>
       <c r="V6" s="5"/>
       <c r="AA6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="13" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="P7" s="5"/>
@@ -1708,11 +1727,11 @@
       <c r="L8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1731,11 +1750,11 @@
       <c r="L9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -1790,11 +1809,11 @@
       <c r="N11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>37</v>
+      <c r="O11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>4</v>
@@ -1926,41 +1945,41 @@
       <c r="AE14" s="5"/>
     </row>
     <row r="15" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="T15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="U15" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="V15" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="W15" s="13" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="U15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="W15" s="12" t="s">
         <v>6</v>
       </c>
       <c r="X15" s="5"/>
@@ -1989,7 +2008,7 @@
       <c r="U16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="V16" s="19" t="s">
+      <c r="V16" s="17" t="s">
         <v>19</v>
       </c>
       <c r="W16" s="5"/>
@@ -1997,9 +2016,9 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
-      <c r="AD16" s="19"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -2018,7 +2037,7 @@
       <c r="U17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="V17" s="19" t="s">
+      <c r="V17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="W17" s="5"/>
@@ -2026,9 +2045,9 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
-      <c r="AB17" s="19"/>
-      <c r="AC17" s="19"/>
-      <c r="AD17" s="19"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -2182,50 +2201,50 @@
       </c>
     </row>
     <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
-      <c r="AB23" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC23" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD23" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE23" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF23" s="14" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD23" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE23" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF23" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2236,7 +2255,7 @@
       </c>
       <c r="C24" s="5"/>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
@@ -2302,7 +2321,7 @@
   <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2329,9 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="22" width="4.5703125" customWidth="1"/>
+    <col min="4" max="19" width="4.5703125" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4.5703125" customWidth="1"/>
     <col min="23" max="23" width="4.42578125" customWidth="1"/>
     <col min="24" max="25" width="4.5703125" customWidth="1"/>
     <col min="26" max="26" width="3.5703125" customWidth="1"/>
@@ -2320,11 +2341,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8">
@@ -2411,15 +2432,16 @@
       <c r="AE1" s="8">
         <v>28</v>
       </c>
+      <c r="AF1" s="18"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -2437,508 +2459,760 @@
       <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="V4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="18"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="V5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="18"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="V6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
     </row>
     <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="18"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+    </row>
+    <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="18"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="18"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="18"/>
+      <c r="AF12" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="U13" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="V13" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="T14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="U13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="V13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="V14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AF14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T15" s="11" t="s">
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="V16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y16" s="5"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="5"/>
-    </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="V17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="W17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB17" s="5"/>
-    </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="18"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -2950,13 +3224,9 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>10</v>
-      </c>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2972,5 +3242,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushing final edition of HW3
</commit_message>
<xml_diff>
--- a/Assignments/HW3_Matrix.xlsx
+++ b/Assignments/HW3_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\WI2019\Architecture\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FC52E3-3660-49CA-8394-07D96D30CCB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2770A5EA-6918-49B3-8C19-B6FF0DB5437F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B - No forward" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="41">
   <si>
     <t>Instruction</t>
   </si>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +299,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,10 +993,14 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="5" t="s">
-        <v>2</v>
+      <c r="P8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>3</v>
@@ -1025,8 +1030,6 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="5"/>
       <c r="S9" s="5" t="s">
         <v>2</v>
       </c>
@@ -1060,8 +1063,6 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5" t="s">
         <v>2</v>
@@ -2320,7 +2321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020A401E-0E1F-4B01-AAD3-33C84EC0B4CF}">
   <dimension ref="A1:AF19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>

</xml_diff>